<commit_message>
home pro type select options added + options added to template
</commit_message>
<xml_diff>
--- a/app/import_homepros_template.xlsx
+++ b/app/import_homepros_template.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\upwork\Firestore-PHP\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E3588B-F33F-4F50-869F-AC148BD32CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB24C11B-8798-4242-BD9A-311A0A47C917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="clients" sheetId="1" r:id="rId1"/>
+    <sheet name="Home_Pros" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
@@ -397,7 +397,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -436,6 +436,11 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{1A3F2301-B021-4087-A79C-E70E33311CA3}">
+      <formula1>"Cleaning,Electrical,Fencing,Handy person,Home Renovation,HVAC,Inspector,Lawncare,Painting,Pest Control,Plumbing,Power Washing,Roofing,Security System,Windows,Other"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>

</xml_diff>